<commit_message>
wtf is cuda on?
</commit_message>
<xml_diff>
--- a/vcpMemory.xlsx
+++ b/vcpMemory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leont\Documents\Spacecraft Attitude Determination\StarTrackSpeed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7D700E-C65B-4CDF-82E3-1D068F336BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D14709-9597-4DCF-918B-E3E98B482FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23640" yWindow="7190" windowWidth="28800" windowHeight="15460" xr2:uid="{1FCA4A27-0538-4455-9757-EDE52F286F7B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1FCA4A27-0538-4455-9757-EDE52F286F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>tidx</t>
   </si>
@@ -134,6 +134,21 @@
   </si>
   <si>
     <t>NEG</t>
+  </si>
+  <si>
+    <t>tid</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>col</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>col2</t>
   </si>
 </sst>
 </file>
@@ -521,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7B253D-C52A-43E9-B5EE-08A7F4D560ED}">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,10 +565,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -615,27 +630,27 @@
       </c>
       <c r="C7">
         <f xml:space="preserve"> B7*$C$4 + $A$4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f xml:space="preserve"> $A$4*3 +B7</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7">
         <f>(MOD(B7+1,3)*$C$4+$A$4)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <f xml:space="preserve"> $A$4*3 +MOD(B7+2,3)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H7">
         <f>(MOD(B7+2,3))*$C$4 + $A$4</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I7">
         <f xml:space="preserve"> $A$4*3 +MOD(B7+1,3)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K7" t="s">
         <v>9</v>
@@ -645,11 +660,11 @@
       </c>
       <c r="M7">
         <f xml:space="preserve"> $A$4*3 +L7</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N7">
         <f xml:space="preserve"> $A$4*3 +L7</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
@@ -661,27 +676,27 @@
       </c>
       <c r="C8">
         <f t="shared" ref="C8:C9" si="0" xml:space="preserve"> B8*$C$4 + $A$4</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <f xml:space="preserve"> $A$4*3 +B8</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F8">
         <f t="shared" ref="F8:F9" si="1">(MOD(B8+1,3)*$C$4+$A$4)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <f t="shared" ref="G8:G9" si="2" xml:space="preserve"> $A$4*3 +MOD(B8+2,3)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <f t="shared" ref="H8:H9" si="3">(MOD(B8+2,3))*$C$4 + $A$4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <f t="shared" ref="I8:I9" si="4" xml:space="preserve"> $A$4*3 +MOD(B8+1,3)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K8" t="s">
         <v>10</v>
@@ -691,11 +706,11 @@
       </c>
       <c r="M8">
         <f t="shared" ref="M8:M9" si="5" xml:space="preserve"> $A$4*3 +L8</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N8">
         <f xml:space="preserve"> $A$4*3 +L8</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
@@ -707,27 +722,27 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <f xml:space="preserve"> $A$4*3 +B9</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H9">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I9">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K9" t="s">
         <v>11</v>
@@ -737,11 +752,11 @@
       </c>
       <c r="M9">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N9">
         <f xml:space="preserve"> $A$4*3 +L9</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
@@ -752,17 +767,31 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.35">
       <c r="C20">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>2</v>
+      </c>
+      <c r="S21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>14</v>
       </c>
@@ -781,8 +810,20 @@
       <c r="K22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="P22">
+        <v>4</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="R22">
+        <v>6</v>
+      </c>
+      <c r="S22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>0</v>
       </c>
@@ -815,7 +856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>3</v>
       </c>
@@ -851,7 +892,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>6</v>
       </c>
@@ -884,7 +925,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.35">
       <c r="F26" s="1" t="s">
         <v>28</v>
       </c>
@@ -911,7 +952,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.35">
       <c r="F27" t="s">
         <v>24</v>
       </c>
@@ -935,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>22</v>
       </c>
@@ -965,7 +1006,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>0</v>
       </c>
@@ -995,7 +1036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>0</v>
       </c>
@@ -1028,7 +1069,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B31">
         <v>0</v>
       </c>
@@ -1058,7 +1099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>1</v>
       </c>
@@ -1066,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>1</v>
       </c>
@@ -1074,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>1</v>
       </c>
@@ -1082,7 +1123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B35">
         <v>2</v>
       </c>
@@ -1090,7 +1131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>2</v>
       </c>
@@ -1098,12 +1139,1180 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37">
         <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="K39">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I42" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J42" s="3">
+        <v>0</v>
+      </c>
+      <c r="K42" s="3">
+        <v>1</v>
+      </c>
+      <c r="L42" s="3">
+        <v>2</v>
+      </c>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O42" s="3">
+        <v>0</v>
+      </c>
+      <c r="P42" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="E44" t="b">
+        <f>AND(B44=C44)</f>
+        <v>1</v>
+      </c>
+      <c r="I44" s="3">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <f>I44*$I$39+$J$42</f>
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <f>I44*$I$39+$K$42</f>
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <f>I44*$I$39+$L$42</f>
+        <v>2</v>
+      </c>
+      <c r="N44" s="3">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <f>$O$42*32+N44</f>
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <f>$P$42*32+N44</f>
+        <v>32</v>
+      </c>
+      <c r="Q44">
+        <f>$Q$42*32+N44</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="b">
+        <f t="shared" ref="E45:E52" si="10">AND(B45=C45)</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="3">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <f>I45*$I$39+$J$42</f>
+        <v>3</v>
+      </c>
+      <c r="K45">
+        <f>I45*$I$39+$K$42</f>
+        <v>4</v>
+      </c>
+      <c r="L45">
+        <f>I45*$I$39+$L$42</f>
+        <v>5</v>
+      </c>
+      <c r="N45" s="3">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <f t="shared" ref="O45:O75" si="11">$O$42*32+N45</f>
+        <v>1</v>
+      </c>
+      <c r="P45">
+        <f t="shared" ref="P45:P75" si="12">$P$42*32+N45</f>
+        <v>33</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" ref="Q45:Q75" si="13">$Q$42*32+N45</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="E46" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I46" s="3">
+        <v>2</v>
+      </c>
+      <c r="J46">
+        <f t="shared" ref="J46:J75" si="14">I46*$I$39+$J$42</f>
+        <v>6</v>
+      </c>
+      <c r="K46">
+        <f t="shared" ref="K46:K75" si="15">I46*$I$39+$K$42</f>
+        <v>7</v>
+      </c>
+      <c r="L46">
+        <f t="shared" ref="L46:L75" si="16">I46*$I$39+$L$42</f>
+        <v>8</v>
+      </c>
+      <c r="N46" s="3">
+        <v>2</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="12"/>
+        <v>34</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="13"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="E47" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I47" s="3">
+        <v>3</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="15"/>
+        <v>10</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="16"/>
+        <v>11</v>
+      </c>
+      <c r="N47" s="3">
+        <v>3</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="12"/>
+        <v>35</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="13"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="E48" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="I48" s="3">
+        <v>4</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="14"/>
+        <v>12</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="15"/>
+        <v>13</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="16"/>
+        <v>14</v>
+      </c>
+      <c r="N48" s="3">
+        <v>4</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="12"/>
+        <v>36</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="E49" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <v>5</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="14"/>
+        <v>15</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="15"/>
+        <v>16</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="16"/>
+        <v>17</v>
+      </c>
+      <c r="N49" s="3">
+        <v>5</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="12"/>
+        <v>37</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="13"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="E50" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <v>6</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="14"/>
+        <v>18</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="15"/>
+        <v>19</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="16"/>
+        <v>20</v>
+      </c>
+      <c r="N50" s="3">
+        <v>6</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="12"/>
+        <v>38</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="13"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I51" s="3">
+        <v>7</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="14"/>
+        <v>21</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="15"/>
+        <v>22</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="16"/>
+        <v>23</v>
+      </c>
+      <c r="N51" s="3">
+        <v>7</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="12"/>
+        <v>39</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="13"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="E52" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="I52" s="3">
+        <v>8</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="14"/>
+        <v>24</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="16"/>
+        <v>26</v>
+      </c>
+      <c r="N52" s="3">
+        <v>8</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="12"/>
+        <v>40</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="13"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I53" s="3">
+        <v>9</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="14"/>
+        <v>27</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="15"/>
+        <v>28</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="16"/>
+        <v>29</v>
+      </c>
+      <c r="N53" s="3">
+        <v>9</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="12"/>
+        <v>41</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="13"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I54" s="3">
+        <v>10</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="14"/>
+        <v>30</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="15"/>
+        <v>31</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="16"/>
+        <v>32</v>
+      </c>
+      <c r="N54" s="3">
+        <v>10</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="11"/>
+        <v>10</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="12"/>
+        <v>42</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="13"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I55" s="3">
+        <v>11</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="14"/>
+        <v>33</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="15"/>
+        <v>34</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="16"/>
+        <v>35</v>
+      </c>
+      <c r="N55" s="3">
+        <v>11</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="11"/>
+        <v>11</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="12"/>
+        <v>43</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I56" s="3">
+        <v>12</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="14"/>
+        <v>36</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="15"/>
+        <v>37</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="16"/>
+        <v>38</v>
+      </c>
+      <c r="N56" s="3">
+        <v>12</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="12"/>
+        <v>44</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="13"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I57" s="3">
+        <v>13</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="14"/>
+        <v>39</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="16"/>
+        <v>41</v>
+      </c>
+      <c r="N57" s="3">
+        <v>13</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="11"/>
+        <v>13</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="12"/>
+        <v>45</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="13"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I58" s="3">
+        <v>14</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="14"/>
+        <v>42</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="15"/>
+        <v>43</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="16"/>
+        <v>44</v>
+      </c>
+      <c r="N58" s="3">
+        <v>14</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="11"/>
+        <v>14</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="12"/>
+        <v>46</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="13"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I59" s="3">
+        <v>15</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="14"/>
+        <v>45</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="15"/>
+        <v>46</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="16"/>
+        <v>47</v>
+      </c>
+      <c r="N59" s="3">
+        <v>15</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="11"/>
+        <v>15</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="12"/>
+        <v>47</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="13"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I60" s="3">
+        <v>16</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="14"/>
+        <v>48</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="15"/>
+        <v>49</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="16"/>
+        <v>50</v>
+      </c>
+      <c r="N60" s="3">
+        <v>16</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="11"/>
+        <v>16</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="12"/>
+        <v>48</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="13"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I61" s="3">
+        <v>17</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="14"/>
+        <v>51</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="15"/>
+        <v>52</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="16"/>
+        <v>53</v>
+      </c>
+      <c r="N61" s="3">
+        <v>17</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="11"/>
+        <v>17</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="12"/>
+        <v>49</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="13"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I62" s="3">
+        <v>18</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="14"/>
+        <v>54</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="15"/>
+        <v>55</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="16"/>
+        <v>56</v>
+      </c>
+      <c r="N62" s="3">
+        <v>18</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="11"/>
+        <v>18</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="12"/>
+        <v>50</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="13"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I63" s="3">
+        <v>19</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="14"/>
+        <v>57</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="15"/>
+        <v>58</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="16"/>
+        <v>59</v>
+      </c>
+      <c r="N63" s="3">
+        <v>19</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="11"/>
+        <v>19</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="12"/>
+        <v>51</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="13"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I64" s="3">
+        <v>20</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="14"/>
+        <v>60</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="15"/>
+        <v>61</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="16"/>
+        <v>62</v>
+      </c>
+      <c r="N64" s="3">
+        <v>20</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="12"/>
+        <v>52</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="13"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I65" s="3">
+        <v>21</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="14"/>
+        <v>63</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="15"/>
+        <v>64</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="16"/>
+        <v>65</v>
+      </c>
+      <c r="N65" s="3">
+        <v>21</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="11"/>
+        <v>21</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="12"/>
+        <v>53</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="13"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I66" s="3">
+        <v>22</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="14"/>
+        <v>66</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="15"/>
+        <v>67</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="16"/>
+        <v>68</v>
+      </c>
+      <c r="N66" s="3">
+        <v>22</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="11"/>
+        <v>22</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="12"/>
+        <v>54</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="13"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I67" s="3">
+        <v>23</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="14"/>
+        <v>69</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="15"/>
+        <v>70</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="16"/>
+        <v>71</v>
+      </c>
+      <c r="N67" s="3">
+        <v>23</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="11"/>
+        <v>23</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="12"/>
+        <v>55</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="13"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I68" s="3">
+        <v>24</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="14"/>
+        <v>72</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="15"/>
+        <v>73</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="16"/>
+        <v>74</v>
+      </c>
+      <c r="N68" s="3">
+        <v>24</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+      <c r="P68">
+        <f t="shared" si="12"/>
+        <v>56</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="13"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I69" s="3">
+        <v>25</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="14"/>
+        <v>75</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="15"/>
+        <v>76</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="16"/>
+        <v>77</v>
+      </c>
+      <c r="N69" s="3">
+        <v>25</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="P69">
+        <f t="shared" si="12"/>
+        <v>57</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" si="13"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I70" s="3">
+        <v>26</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="14"/>
+        <v>78</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="15"/>
+        <v>79</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="16"/>
+        <v>80</v>
+      </c>
+      <c r="N70" s="3">
+        <v>26</v>
+      </c>
+      <c r="O70">
+        <f t="shared" si="11"/>
+        <v>26</v>
+      </c>
+      <c r="P70">
+        <f t="shared" si="12"/>
+        <v>58</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" si="13"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I71" s="3">
+        <v>27</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="14"/>
+        <v>81</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="15"/>
+        <v>82</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="16"/>
+        <v>83</v>
+      </c>
+      <c r="N71" s="3">
+        <v>27</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="11"/>
+        <v>27</v>
+      </c>
+      <c r="P71">
+        <f t="shared" si="12"/>
+        <v>59</v>
+      </c>
+      <c r="Q71">
+        <f t="shared" si="13"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I72" s="3">
+        <v>28</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="14"/>
+        <v>84</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="15"/>
+        <v>85</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="16"/>
+        <v>86</v>
+      </c>
+      <c r="N72" s="3">
+        <v>28</v>
+      </c>
+      <c r="O72">
+        <f t="shared" si="11"/>
+        <v>28</v>
+      </c>
+      <c r="P72">
+        <f t="shared" si="12"/>
+        <v>60</v>
+      </c>
+      <c r="Q72">
+        <f t="shared" si="13"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I73" s="3">
+        <v>29</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="14"/>
+        <v>87</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="15"/>
+        <v>88</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="16"/>
+        <v>89</v>
+      </c>
+      <c r="N73" s="3">
+        <v>29</v>
+      </c>
+      <c r="O73">
+        <f t="shared" si="11"/>
+        <v>29</v>
+      </c>
+      <c r="P73">
+        <f t="shared" si="12"/>
+        <v>61</v>
+      </c>
+      <c r="Q73">
+        <f t="shared" si="13"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I74" s="3">
+        <v>30</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="14"/>
+        <v>90</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="15"/>
+        <v>91</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="16"/>
+        <v>92</v>
+      </c>
+      <c r="N74" s="3">
+        <v>30</v>
+      </c>
+      <c r="O74">
+        <f t="shared" si="11"/>
+        <v>30</v>
+      </c>
+      <c r="P74">
+        <f t="shared" si="12"/>
+        <v>62</v>
+      </c>
+      <c r="Q74">
+        <f t="shared" si="13"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="75" spans="9:17" x14ac:dyDescent="0.35">
+      <c r="I75" s="3">
+        <v>31</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="14"/>
+        <v>93</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="15"/>
+        <v>94</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="16"/>
+        <v>95</v>
+      </c>
+      <c r="N75" s="3">
+        <v>31</v>
+      </c>
+      <c r="O75">
+        <f t="shared" si="11"/>
+        <v>31</v>
+      </c>
+      <c r="P75">
+        <f t="shared" si="12"/>
+        <v>63</v>
+      </c>
+      <c r="Q75">
+        <f t="shared" si="13"/>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>